<commit_message>
Load the population-weighted summary table by group (on-track, off-track)
</commit_message>
<xml_diff>
--- a/output/un_population.xlsx
+++ b/output/un_population.xlsx
@@ -385,15 +385,11 @@
           <t>BDI</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12889.575999999999</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>439.64800000000002</t>
-        </is>
+      <c r="B2">
+        <v>12889.576</v>
+      </c>
+      <c r="C2">
+        <v>439.648</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -407,15 +403,11 @@
           <t>COM</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>836.774</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>24.201000000000001</t>
-        </is>
+      <c r="B3">
+        <v>836.774</v>
+      </c>
+      <c r="C3">
+        <v>24.201</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -429,15 +421,11 @@
           <t>DJI</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1120.8489999999999</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>24.548999999999999</t>
-        </is>
+      <c r="B4">
+        <v>1120.849</v>
+      </c>
+      <c r="C4">
+        <v>24.549</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -451,15 +439,11 @@
           <t>ERI</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>3684.0320000000002</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>104.98099999999999</t>
-        </is>
+      <c r="B5">
+        <v>3684.032</v>
+      </c>
+      <c r="C5">
+        <v>104.981</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -473,15 +457,11 @@
           <t>ETH</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>123379.924</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>3928.4450000000002</t>
-        </is>
+      <c r="B6">
+        <v>123379.924</v>
+      </c>
+      <c r="C6">
+        <v>3928.445</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -495,15 +475,11 @@
           <t>KEN</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>54027.487000000001</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1488.394</t>
-        </is>
+      <c r="B7">
+        <v>54027.487</v>
+      </c>
+      <c r="C7">
+        <v>1488.394</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -517,15 +493,11 @@
           <t>MDG</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>29611.714</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>906.13</t>
-        </is>
+      <c r="B8">
+        <v>29611.714</v>
+      </c>
+      <c r="C8">
+        <v>906.13</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -539,15 +511,11 @@
           <t>MWI</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>20405.316999999999</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>665.678</t>
-        </is>
+      <c r="B9">
+        <v>20405.317</v>
+      </c>
+      <c r="C9">
+        <v>665.678</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -561,15 +529,11 @@
           <t>MUS</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1299.4690000000001</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>13.266</t>
-        </is>
+      <c r="B10">
+        <v>1299.469</v>
+      </c>
+      <c r="C10">
+        <v>13.266</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -583,15 +547,11 @@
           <t>MYT</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>326.101</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>10.754</t>
-        </is>
+      <c r="B11">
+        <v>326.101</v>
+      </c>
+      <c r="C11">
+        <v>10.754</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -605,15 +565,11 @@
           <t>MOZ</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>32969.517999999996</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>1191.1469999999999</t>
-        </is>
+      <c r="B12">
+        <v>32969.518</v>
+      </c>
+      <c r="C12">
+        <v>1191.147</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -627,15 +583,11 @@
           <t>REU</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>974.05200000000002</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>13.968999999999999</t>
-        </is>
+      <c r="B13">
+        <v>974.052</v>
+      </c>
+      <c r="C13">
+        <v>13.969</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -649,15 +601,11 @@
           <t>RWA</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>13776.698</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>406.214</t>
-        </is>
+      <c r="B14">
+        <v>13776.698</v>
+      </c>
+      <c r="C14">
+        <v>406.214</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -671,15 +619,11 @@
           <t>SYC</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>107.11799999999999</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>1.611</t>
-        </is>
+      <c r="B15">
+        <v>107.118</v>
+      </c>
+      <c r="C15">
+        <v>1.611</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -693,15 +637,11 @@
           <t>SOM</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>17597.510999999999</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>759.04399999999998</t>
-        </is>
+      <c r="B16">
+        <v>17597.511</v>
+      </c>
+      <c r="C16">
+        <v>759.044</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -715,15 +655,11 @@
           <t>SSD</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>10913.164000000001</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>315.39</t>
-        </is>
+      <c r="B17">
+        <v>10913.164</v>
+      </c>
+      <c r="C17">
+        <v>315.39</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -737,15 +673,11 @@
           <t>UGA</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>47249.584999999999</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1713.605</t>
-        </is>
+      <c r="B18">
+        <v>47249.585</v>
+      </c>
+      <c r="C18">
+        <v>1713.605</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -759,15 +691,11 @@
           <t>TZA</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>65497.748</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2346.8209999999999</t>
-        </is>
+      <c r="B19">
+        <v>65497.748</v>
+      </c>
+      <c r="C19">
+        <v>2346.821</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -781,15 +709,11 @@
           <t>ZMB</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>20017.674999999999</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>683.35500000000002</t>
-        </is>
+      <c r="B20">
+        <v>20017.675</v>
+      </c>
+      <c r="C20">
+        <v>683.355</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -803,15 +727,11 @@
           <t>ZWE</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>16320.537</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>491.19499999999999</t>
-        </is>
+      <c r="B21">
+        <v>16320.537</v>
+      </c>
+      <c r="C21">
+        <v>491.195</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -825,15 +745,11 @@
           <t>AGO</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>35588.987000000001</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>1359.723</t>
-        </is>
+      <c r="B22">
+        <v>35588.987</v>
+      </c>
+      <c r="C22">
+        <v>1359.723</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -847,15 +763,11 @@
           <t>CMR</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>27914.536</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>959.096</t>
-        </is>
+      <c r="B23">
+        <v>27914.536</v>
+      </c>
+      <c r="C23">
+        <v>959.096</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -869,15 +781,11 @@
           <t>CAF</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>5579.1440000000002</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>236.643</t>
-        </is>
+      <c r="B24">
+        <v>5579.144</v>
+      </c>
+      <c r="C24">
+        <v>236.643</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -891,15 +799,11 @@
           <t>TCD</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>17723.314999999999</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>765.64800000000002</t>
-        </is>
+      <c r="B25">
+        <v>17723.315</v>
+      </c>
+      <c r="C25">
+        <v>765.648</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -913,15 +817,11 @@
           <t>COG</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>5970.424</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>180.17500000000001</t>
-        </is>
+      <c r="B26">
+        <v>5970.424</v>
+      </c>
+      <c r="C26">
+        <v>180.175</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -935,15 +835,11 @@
           <t>COD</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>99010.212</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>4133.9870000000001</t>
-        </is>
+      <c r="B27">
+        <v>99010.212</v>
+      </c>
+      <c r="C27">
+        <v>4133.987</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -957,15 +853,11 @@
           <t>GNQ</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>1674.9079999999999</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>49.963999999999999</t>
-        </is>
+      <c r="B28">
+        <v>1674.908</v>
+      </c>
+      <c r="C28">
+        <v>49.964</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -979,15 +871,11 @@
           <t>GAB</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>2388.9920000000002</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>64.022000000000006</t>
-        </is>
+      <c r="B29">
+        <v>2388.992</v>
+      </c>
+      <c r="C29">
+        <v>64.02200000000001</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1001,15 +889,11 @@
           <t>STP</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>227.38</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>6.37</t>
-        </is>
+      <c r="B30">
+        <v>227.38</v>
+      </c>
+      <c r="C30">
+        <v>6.37</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1023,15 +907,11 @@
           <t>DZA</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>44903.224999999999</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>923.64800000000002</t>
-        </is>
+      <c r="B31">
+        <v>44903.225</v>
+      </c>
+      <c r="C31">
+        <v>923.648</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1045,15 +925,11 @@
           <t>EGY</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>110990.103</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>2453.9409999999998</t>
-        </is>
+      <c r="B32">
+        <v>110990.103</v>
+      </c>
+      <c r="C32">
+        <v>2453.941</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1067,15 +943,11 @@
           <t>LBY</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>6812.3410000000003</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>117.846</t>
-        </is>
+      <c r="B33">
+        <v>6812.341</v>
+      </c>
+      <c r="C33">
+        <v>117.846</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1089,15 +961,11 @@
           <t>MAR</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>37457.970999999998</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>643.10900000000004</t>
-        </is>
+      <c r="B34">
+        <v>37457.971</v>
+      </c>
+      <c r="C34">
+        <v>643.109</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1111,15 +979,11 @@
           <t>SDN</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>46874.203999999998</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>1548.473</t>
-        </is>
+      <c r="B35">
+        <v>46874.204</v>
+      </c>
+      <c r="C35">
+        <v>1548.473</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1133,15 +997,11 @@
           <t>TUN</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>12356.117</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>192.75899999999999</t>
-        </is>
+      <c r="B36">
+        <v>12356.117</v>
+      </c>
+      <c r="C36">
+        <v>192.759</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1155,15 +1015,11 @@
           <t>ESH</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>575.98599999999999</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>9.3559999999999999</t>
-        </is>
+      <c r="B37">
+        <v>575.986</v>
+      </c>
+      <c r="C37">
+        <v>9.356</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1177,15 +1033,11 @@
           <t>BWA</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>2630.2959999999998</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>60.554000000000002</t>
-        </is>
+      <c r="B38">
+        <v>2630.296</v>
+      </c>
+      <c r="C38">
+        <v>60.554</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1199,15 +1051,11 @@
           <t>SWZ</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>1201.67</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>28.475999999999999</t>
-        </is>
+      <c r="B39">
+        <v>1201.67</v>
+      </c>
+      <c r="C39">
+        <v>28.476</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1221,15 +1069,11 @@
           <t>LSO</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>2305.8249999999998</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>59.49</t>
-        </is>
+      <c r="B40">
+        <v>2305.825</v>
+      </c>
+      <c r="C40">
+        <v>59.49</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1243,15 +1087,11 @@
           <t>NAM</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2567.0120000000002</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>69.156999999999996</t>
-        </is>
+      <c r="B41">
+        <v>2567.012</v>
+      </c>
+      <c r="C41">
+        <v>69.157</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1265,15 +1105,11 @@
           <t>ZAF</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>59893.885000000002</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>1155.8579999999999</t>
-        </is>
+      <c r="B42">
+        <v>59893.885</v>
+      </c>
+      <c r="C42">
+        <v>1155.858</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1287,15 +1123,11 @@
           <t>BEN</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>13352.864</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>481.71499999999997</t>
-        </is>
+      <c r="B43">
+        <v>13352.864</v>
+      </c>
+      <c r="C43">
+        <v>481.715</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1309,15 +1141,11 @@
           <t>BFA</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>22673.761999999999</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>793.03099999999995</t>
-        </is>
+      <c r="B44">
+        <v>22673.762</v>
+      </c>
+      <c r="C44">
+        <v>793.0309999999999</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1331,15 +1159,11 @@
           <t>CPV</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>593.149</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>9.9079999999999995</t>
-        </is>
+      <c r="B45">
+        <v>593.149</v>
+      </c>
+      <c r="C45">
+        <v>9.907999999999999</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1353,15 +1177,11 @@
           <t>CIV</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>28160.542000000001</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>943.13300000000004</t>
-        </is>
+      <c r="B46">
+        <v>28160.542</v>
+      </c>
+      <c r="C46">
+        <v>943.133</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1375,15 +1195,11 @@
           <t>GMB</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2705.9920000000002</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>88.534999999999997</t>
-        </is>
+      <c r="B47">
+        <v>2705.992</v>
+      </c>
+      <c r="C47">
+        <v>88.535</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1397,15 +1213,11 @@
           <t>GHA</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>33475.870000000003</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>906.67700000000002</t>
-        </is>
+      <c r="B48">
+        <v>33475.87</v>
+      </c>
+      <c r="C48">
+        <v>906.677</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1419,15 +1231,11 @@
           <t>GIN</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>13859.341</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>469.31099999999998</t>
-        </is>
+      <c r="B49">
+        <v>13859.341</v>
+      </c>
+      <c r="C49">
+        <v>469.311</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1441,15 +1249,11 @@
           <t>GNB</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>2105.5659999999998</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>64.478999999999999</t>
-        </is>
+      <c r="B50">
+        <v>2105.566</v>
+      </c>
+      <c r="C50">
+        <v>64.479</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1463,15 +1267,11 @@
           <t>LBR</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>5302.6809999999996</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>164.452</t>
-        </is>
+      <c r="B51">
+        <v>5302.681</v>
+      </c>
+      <c r="C51">
+        <v>164.452</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1485,15 +1285,11 @@
           <t>MLI</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>22593.59</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>932.31700000000001</t>
-        </is>
+      <c r="B52">
+        <v>22593.59</v>
+      </c>
+      <c r="C52">
+        <v>932.317</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1507,15 +1303,11 @@
           <t>MRT</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>4736.1390000000001</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>156.047</t>
-        </is>
+      <c r="B53">
+        <v>4736.139</v>
+      </c>
+      <c r="C53">
+        <v>156.047</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1529,15 +1321,11 @@
           <t>NER</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>26207.976999999999</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>1180.654</t>
-        </is>
+      <c r="B54">
+        <v>26207.977</v>
+      </c>
+      <c r="C54">
+        <v>1180.654</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1551,15 +1339,11 @@
           <t>NGA</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>218541.212</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>8002.7579999999998</t>
-        </is>
+      <c r="B55">
+        <v>218541.212</v>
+      </c>
+      <c r="C55">
+        <v>8002.758</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1573,15 +1357,11 @@
           <t>SHN</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>5.3739999999999997</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>0.04</t>
-        </is>
+      <c r="B56">
+        <v>5.374</v>
+      </c>
+      <c r="C56">
+        <v>0.04</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1595,15 +1375,11 @@
           <t>SEN</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>17316.449000000001</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>555.69600000000003</t>
-        </is>
+      <c r="B57">
+        <v>17316.449</v>
+      </c>
+      <c r="C57">
+        <v>555.696</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1617,15 +1393,11 @@
           <t>SLE</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>8605.7180000000008</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>265.02300000000002</t>
-        </is>
+      <c r="B58">
+        <v>8605.718000000001</v>
+      </c>
+      <c r="C58">
+        <v>265.023</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1639,15 +1411,11 @@
           <t>TGO</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>8848.6990000000005</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>278.61799999999999</t>
-        </is>
+      <c r="B59">
+        <v>8848.699000000001</v>
+      </c>
+      <c r="C59">
+        <v>278.618</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1661,15 +1429,11 @@
           <t>KAZ</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>19397.998</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>402.51100000000002</t>
-        </is>
+      <c r="B60">
+        <v>19397.998</v>
+      </c>
+      <c r="C60">
+        <v>402.511</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1683,15 +1447,11 @@
           <t>KGZ</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>6630.6229999999996</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>154.761</t>
-        </is>
+      <c r="B61">
+        <v>6630.623</v>
+      </c>
+      <c r="C61">
+        <v>154.761</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1705,15 +1465,11 @@
           <t>TJK</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>9952.7870000000003</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>259.27600000000001</t>
-        </is>
+      <c r="B62">
+        <v>9952.787</v>
+      </c>
+      <c r="C62">
+        <v>259.276</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1727,15 +1483,11 @@
           <t>TKM</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>6430.77</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>133.49100000000001</t>
-        </is>
+      <c r="B63">
+        <v>6430.77</v>
+      </c>
+      <c r="C63">
+        <v>133.491</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1749,15 +1501,11 @@
           <t>UZB</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>34627.652000000002</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>776.81500000000005</t>
-        </is>
+      <c r="B64">
+        <v>34627.652</v>
+      </c>
+      <c r="C64">
+        <v>776.8150000000001</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1771,15 +1519,11 @@
           <t>CHN</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>1425887.3370000001</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>10757.794</t>
-        </is>
+      <c r="B65">
+        <v>1425887.337</v>
+      </c>
+      <c r="C65">
+        <v>10757.794</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1793,15 +1537,11 @@
           <t>HKG</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7488.8649999999998</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>41.923000000000002</t>
-        </is>
+      <c r="B66">
+        <v>7488.865</v>
+      </c>
+      <c r="C66">
+        <v>41.923</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1815,15 +1555,11 @@
           <t>MAC</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>695.16800000000001</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>6.9569999999999999</t>
-        </is>
+      <c r="B67">
+        <v>695.168</v>
+      </c>
+      <c r="C67">
+        <v>6.957</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1837,15 +1573,11 @@
           <t>TWN</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>23893.394</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>186.24100000000001</t>
-        </is>
+      <c r="B68">
+        <v>23893.394</v>
+      </c>
+      <c r="C68">
+        <v>186.241</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1859,15 +1591,11 @@
           <t>PRK</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>26069.416000000001</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>340.40699999999998</t>
-        </is>
+      <c r="B69">
+        <v>26069.416</v>
+      </c>
+      <c r="C69">
+        <v>340.407</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1881,15 +1609,11 @@
           <t>JPN</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>123951.692</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>814.70500000000004</t>
-        </is>
+      <c r="B70">
+        <v>123951.692</v>
+      </c>
+      <c r="C70">
+        <v>814.705</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1903,15 +1627,11 @@
           <t>MNG</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>3398.366</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>69.480999999999995</t>
-        </is>
+      <c r="B71">
+        <v>3398.366</v>
+      </c>
+      <c r="C71">
+        <v>69.48099999999999</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1925,15 +1645,11 @@
           <t>KOR</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>51815.81</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>285.68599999999998</t>
-        </is>
+      <c r="B72">
+        <v>51815.81</v>
+      </c>
+      <c r="C72">
+        <v>285.686</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1947,15 +1663,11 @@
           <t>AFG</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>41128.771000000001</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>1446.6990000000001</t>
-        </is>
+      <c r="B73">
+        <v>41128.771</v>
+      </c>
+      <c r="C73">
+        <v>1446.699</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1969,15 +1681,11 @@
           <t>BGD</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>171186.372</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>2994.9659999999999</t>
-        </is>
+      <c r="B74">
+        <v>171186.372</v>
+      </c>
+      <c r="C74">
+        <v>2994.966</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1991,15 +1699,11 @@
           <t>BTN</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>782.45500000000004</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>9.6479999999999997</t>
-        </is>
+      <c r="B75">
+        <v>782.455</v>
+      </c>
+      <c r="C75">
+        <v>9.648</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2013,15 +1717,11 @@
           <t>IND</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>1417173.173</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>23056.026999999998</t>
-        </is>
+      <c r="B76">
+        <v>1417173.173</v>
+      </c>
+      <c r="C76">
+        <v>23056.027</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2035,15 +1735,11 @@
           <t>IRN</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>88550.57</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>1172.7090000000001</t>
-        </is>
+      <c r="B77">
+        <v>88550.57000000001</v>
+      </c>
+      <c r="C77">
+        <v>1172.709</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2057,15 +1753,11 @@
           <t>MDV</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>523.78700000000003</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>7.1970000000000001</t>
-        </is>
+      <c r="B78">
+        <v>523.787</v>
+      </c>
+      <c r="C78">
+        <v>7.197</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2079,15 +1771,11 @@
           <t>NPL</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>30547.58</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>616.65700000000004</t>
-        </is>
+      <c r="B79">
+        <v>30547.58</v>
+      </c>
+      <c r="C79">
+        <v>616.657</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2101,15 +1789,11 @@
           <t>PAK</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>235824.86199999999</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>6424.9440000000004</t>
-        </is>
+      <c r="B80">
+        <v>235824.862</v>
+      </c>
+      <c r="C80">
+        <v>6424.944</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2123,15 +1807,11 @@
           <t>LKA</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>21832.143</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>301.38299999999998</t>
-        </is>
+      <c r="B81">
+        <v>21832.143</v>
+      </c>
+      <c r="C81">
+        <v>301.383</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2145,15 +1825,11 @@
           <t>BRN</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>449.00200000000001</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>6.0579999999999998</t>
-        </is>
+      <c r="B82">
+        <v>449.002</v>
+      </c>
+      <c r="C82">
+        <v>6.058</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2167,15 +1843,11 @@
           <t>KHM</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>16767.842000000001</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>318.33499999999998</t>
-        </is>
+      <c r="B83">
+        <v>16767.842</v>
+      </c>
+      <c r="C83">
+        <v>318.335</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2189,15 +1861,11 @@
           <t>IDN</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>275501.33899999998</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>4462.2120000000004</t>
-        </is>
+      <c r="B84">
+        <v>275501.339</v>
+      </c>
+      <c r="C84">
+        <v>4462.212</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2211,15 +1879,11 @@
           <t>LAO</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>7529.4750000000004</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>161.68199999999999</t>
-        </is>
+      <c r="B85">
+        <v>7529.475</v>
+      </c>
+      <c r="C85">
+        <v>161.682</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2233,15 +1897,11 @@
           <t>MYS</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>33938.220999999998</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>509.23200000000003</t>
-        </is>
+      <c r="B86">
+        <v>33938.221</v>
+      </c>
+      <c r="C86">
+        <v>509.232</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2255,15 +1915,11 @@
           <t>MMR</t>
         </is>
       </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>54179.305999999997</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>912.25199999999995</t>
-        </is>
+      <c r="B87">
+        <v>54179.306</v>
+      </c>
+      <c r="C87">
+        <v>912.252</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2277,15 +1933,11 @@
           <t>PHL</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>115559.00900000001</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>2499.0810000000001</t>
-        </is>
+      <c r="B88">
+        <v>115559.009</v>
+      </c>
+      <c r="C88">
+        <v>2499.081</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2299,15 +1951,11 @@
           <t>SGP</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>5975.6890000000003</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>42.332999999999998</t>
-        </is>
+      <c r="B89">
+        <v>5975.689</v>
+      </c>
+      <c r="C89">
+        <v>42.333</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2321,15 +1969,11 @@
           <t>THA</t>
         </is>
       </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>71697.03</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>631.23900000000003</t>
-        </is>
+      <c r="B90">
+        <v>71697.03</v>
+      </c>
+      <c r="C90">
+        <v>631.239</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2343,15 +1987,11 @@
           <t>TLS</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>1341.296</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>33.073999999999998</t>
-        </is>
+      <c r="B91">
+        <v>1341.296</v>
+      </c>
+      <c r="C91">
+        <v>33.074</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2365,15 +2005,11 @@
           <t>VNM</t>
         </is>
       </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>98186.856</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>1442.809</t>
-        </is>
+      <c r="B92">
+        <v>98186.856</v>
+      </c>
+      <c r="C92">
+        <v>1442.809</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2387,15 +2023,11 @@
           <t>ARM</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>2780.4690000000001</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>32.555999999999997</t>
-        </is>
+      <c r="B93">
+        <v>2780.469</v>
+      </c>
+      <c r="C93">
+        <v>32.556</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2409,15 +2041,11 @@
           <t>AZE</t>
         </is>
       </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>10358.074000000001</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>123.673</t>
-        </is>
+      <c r="B94">
+        <v>10358.074</v>
+      </c>
+      <c r="C94">
+        <v>123.673</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2431,15 +2059,11 @@
           <t>BHR</t>
         </is>
       </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>1472.2329999999999</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>16.861000000000001</t>
-        </is>
+      <c r="B95">
+        <v>1472.233</v>
+      </c>
+      <c r="C95">
+        <v>16.861</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2453,15 +2077,11 @@
           <t>CYP</t>
         </is>
       </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>1251.4880000000001</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>12.516999999999999</t>
-        </is>
+      <c r="B96">
+        <v>1251.488</v>
+      </c>
+      <c r="C96">
+        <v>12.517</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2475,15 +2095,11 @@
           <t>GEO</t>
         </is>
       </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>3744.3850000000002</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>49.106000000000002</t>
-        </is>
+      <c r="B97">
+        <v>3744.385</v>
+      </c>
+      <c r="C97">
+        <v>49.106</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2497,15 +2113,11 @@
           <t>IRQ</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>44496.122000000003</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>1203.1880000000001</t>
-        </is>
+      <c r="B98">
+        <v>44496.122</v>
+      </c>
+      <c r="C98">
+        <v>1203.188</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2519,15 +2131,11 @@
           <t>ISR</t>
         </is>
       </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>9038.3089999999993</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>174.67500000000001</t>
-        </is>
+      <c r="B99">
+        <v>9038.308999999999</v>
+      </c>
+      <c r="C99">
+        <v>174.675</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2541,15 +2149,11 @@
           <t>JOR</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>11285.869000000001</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>245.48400000000001</t>
-        </is>
+      <c r="B100">
+        <v>11285.869</v>
+      </c>
+      <c r="C100">
+        <v>245.484</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2563,15 +2167,11 @@
           <t>KWT</t>
         </is>
       </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>4268.8729999999996</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>41.456000000000003</t>
-        </is>
+      <c r="B101">
+        <v>4268.873</v>
+      </c>
+      <c r="C101">
+        <v>41.456</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2585,15 +2185,11 @@
           <t>LBN</t>
         </is>
       </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>5489.7389999999996</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>81.179000000000002</t>
-        </is>
+      <c r="B102">
+        <v>5489.739</v>
+      </c>
+      <c r="C102">
+        <v>81.179</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2607,15 +2203,11 @@
           <t>OMN</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>4576.2979999999998</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>81.043000000000006</t>
-        </is>
+      <c r="B103">
+        <v>4576.298</v>
+      </c>
+      <c r="C103">
+        <v>81.04300000000001</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2629,15 +2221,11 @@
           <t>QAT</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>2695.1219999999998</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>24.497</t>
-        </is>
+      <c r="B104">
+        <v>2695.122</v>
+      </c>
+      <c r="C104">
+        <v>24.497</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -2651,15 +2239,11 @@
           <t>SAU</t>
         </is>
       </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>36408.82</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>615.69000000000005</t>
-        </is>
+      <c r="B105">
+        <v>36408.82</v>
+      </c>
+      <c r="C105">
+        <v>615.6900000000001</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -2673,15 +2257,11 @@
           <t>PSE</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>5250.0720000000001</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>145.44900000000001</t>
-        </is>
+      <c r="B106">
+        <v>5250.072</v>
+      </c>
+      <c r="C106">
+        <v>145.449</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2695,15 +2275,11 @@
           <t>SYR</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>22125.249</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>446.85899999999998</t>
-        </is>
+      <c r="B107">
+        <v>22125.249</v>
+      </c>
+      <c r="C107">
+        <v>446.859</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2717,15 +2293,11 @@
           <t>TUR</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>85341.240999999995</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>1236.9000000000001</t>
-        </is>
+      <c r="B108">
+        <v>85341.24099999999</v>
+      </c>
+      <c r="C108">
+        <v>1236.9</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -2739,15 +2311,11 @@
           <t>ARE</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>9441.1290000000008</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>93.343000000000004</t>
-        </is>
+      <c r="B109">
+        <v>9441.129000000001</v>
+      </c>
+      <c r="C109">
+        <v>93.343</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -2761,15 +2329,11 @@
           <t>YEM</t>
         </is>
       </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>33696.614000000001</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>1008.643</t>
-        </is>
+      <c r="B110">
+        <v>33696.614</v>
+      </c>
+      <c r="C110">
+        <v>1008.643</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -2783,15 +2347,11 @@
           <t>BLR</t>
         </is>
       </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>9534.9539999999997</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>87.251999999999995</t>
-        </is>
+      <c r="B111">
+        <v>9534.954</v>
+      </c>
+      <c r="C111">
+        <v>87.252</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -2805,15 +2365,11 @@
           <t>BGR</t>
         </is>
       </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>6781.9530000000004</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>56.662999999999997</t>
-        </is>
+      <c r="B112">
+        <v>6781.953</v>
+      </c>
+      <c r="C112">
+        <v>56.663</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -2827,15 +2383,11 @@
           <t>CZE</t>
         </is>
       </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>10493.986000000001</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>101.55500000000001</t>
-        </is>
+      <c r="B113">
+        <v>10493.986</v>
+      </c>
+      <c r="C113">
+        <v>101.555</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -2849,15 +2401,11 @@
           <t>HUN</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>9967.3080000000009</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>91.370999999999995</t>
-        </is>
+      <c r="B114">
+        <v>9967.308000000001</v>
+      </c>
+      <c r="C114">
+        <v>91.371</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2871,15 +2419,11 @@
           <t>POL</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>39857.144999999997</t>
-        </is>
-      </c>
-      <c r="C115" t="inlineStr">
-        <is>
-          <t>353.84</t>
-        </is>
+      <c r="B115">
+        <v>39857.145</v>
+      </c>
+      <c r="C115">
+        <v>353.84</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -2893,15 +2437,11 @@
           <t>MDA</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>3272.9960000000001</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>36.942999999999998</t>
-        </is>
+      <c r="B116">
+        <v>3272.996</v>
+      </c>
+      <c r="C116">
+        <v>36.943</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -2915,15 +2455,11 @@
           <t>ROU</t>
         </is>
       </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>19659.267</t>
-        </is>
-      </c>
-      <c r="C117" t="inlineStr">
-        <is>
-          <t>191.76300000000001</t>
-        </is>
+      <c r="B117">
+        <v>19659.267</v>
+      </c>
+      <c r="C117">
+        <v>191.763</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -2937,15 +2473,11 @@
           <t>RUS</t>
         </is>
       </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>144713.31400000001</t>
-        </is>
-      </c>
-      <c r="C118" t="inlineStr">
-        <is>
-          <t>1375.808</t>
-        </is>
+      <c r="B118">
+        <v>144713.314</v>
+      </c>
+      <c r="C118">
+        <v>1375.808</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -2959,15 +2491,11 @@
           <t>SVK</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>5643.4530000000004</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>53.356999999999999</t>
-        </is>
+      <c r="B119">
+        <v>5643.453</v>
+      </c>
+      <c r="C119">
+        <v>53.357</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -2981,15 +2509,11 @@
           <t>UKR</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>39701.739000000001</t>
-        </is>
-      </c>
-      <c r="C120" t="inlineStr">
-        <is>
-          <t>329.61799999999999</t>
-        </is>
+      <c r="B120">
+        <v>39701.739</v>
+      </c>
+      <c r="C120">
+        <v>329.618</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -3003,15 +2527,11 @@
           <t>DNK</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>5882.2610000000004</t>
-        </is>
-      </c>
-      <c r="C121" t="inlineStr">
-        <is>
-          <t>64.106999999999999</t>
-        </is>
+      <c r="B121">
+        <v>5882.261</v>
+      </c>
+      <c r="C121">
+        <v>64.107</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -3025,15 +2545,11 @@
           <t>EST</t>
         </is>
       </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>1326.0619999999999</t>
-        </is>
-      </c>
-      <c r="C122" t="inlineStr">
-        <is>
-          <t>13.422000000000001</t>
-        </is>
+      <c r="B122">
+        <v>1326.062</v>
+      </c>
+      <c r="C122">
+        <v>13.422</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -3047,15 +2563,11 @@
           <t>FRO</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>53.09</t>
-        </is>
-      </c>
-      <c r="C123" t="inlineStr">
-        <is>
-          <t>0.80100000000000005</t>
-        </is>
+      <c r="B123">
+        <v>53.09</v>
+      </c>
+      <c r="C123">
+        <v>0.801</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -3069,15 +2581,11 @@
           <t>FIN</t>
         </is>
       </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>5540.7449999999999</t>
-        </is>
-      </c>
-      <c r="C124" t="inlineStr">
-        <is>
-          <t>47.136000000000003</t>
-        </is>
+      <c r="B124">
+        <v>5540.745</v>
+      </c>
+      <c r="C124">
+        <v>47.136</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -3091,15 +2599,11 @@
           <t>GGY</t>
         </is>
       </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>63.301000000000002</t>
-        </is>
-      </c>
-      <c r="C125" t="inlineStr">
-        <is>
-          <t>0.622</t>
-        </is>
+      <c r="B125">
+        <v>63.301</v>
+      </c>
+      <c r="C125">
+        <v>0.622</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -3113,15 +2617,11 @@
           <t>ISL</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>372.899</t>
-        </is>
-      </c>
-      <c r="C126" t="inlineStr">
-        <is>
-          <t>4.5679999999999996</t>
-        </is>
+      <c r="B126">
+        <v>372.899</v>
+      </c>
+      <c r="C126">
+        <v>4.568</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -3135,15 +2635,11 @@
           <t>IRL</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>5023.1090000000004</t>
-        </is>
-      </c>
-      <c r="C127" t="inlineStr">
-        <is>
-          <t>57.561</t>
-        </is>
+      <c r="B127">
+        <v>5023.109</v>
+      </c>
+      <c r="C127">
+        <v>57.561</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -3157,15 +2653,11 @@
           <t>IMN</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>84.519000000000005</t>
-        </is>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>0.72399999999999998</t>
-        </is>
+      <c r="B128">
+        <v>84.51900000000001</v>
+      </c>
+      <c r="C128">
+        <v>0.724</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -3179,15 +2671,11 @@
           <t>JEY</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>110.77800000000001</t>
-        </is>
-      </c>
-      <c r="C129" t="inlineStr">
-        <is>
-          <t>1.157</t>
-        </is>
+      <c r="B129">
+        <v>110.778</v>
+      </c>
+      <c r="C129">
+        <v>1.157</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
@@ -3201,15 +2689,11 @@
           <t>LVA</t>
         </is>
       </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>1850.6510000000001</t>
-        </is>
-      </c>
-      <c r="C130" t="inlineStr">
-        <is>
-          <t>16.530999999999999</t>
-        </is>
+      <c r="B130">
+        <v>1850.651</v>
+      </c>
+      <c r="C130">
+        <v>16.531</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
@@ -3223,15 +2707,11 @@
           <t>LTU</t>
         </is>
       </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>2750.0549999999998</t>
-        </is>
-      </c>
-      <c r="C131" t="inlineStr">
-        <is>
-          <t>26.206</t>
-        </is>
+      <c r="B131">
+        <v>2750.055</v>
+      </c>
+      <c r="C131">
+        <v>26.206</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
@@ -3245,15 +2725,11 @@
           <t>NOR</t>
         </is>
       </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>5434.3190000000004</t>
-        </is>
-      </c>
-      <c r="C132" t="inlineStr">
-        <is>
-          <t>53.988</t>
-        </is>
+      <c r="B132">
+        <v>5434.319</v>
+      </c>
+      <c r="C132">
+        <v>53.988</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
@@ -3267,15 +2743,11 @@
           <t>SWE</t>
         </is>
       </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>10549.347</t>
-        </is>
-      </c>
-      <c r="C133" t="inlineStr">
-        <is>
-          <t>114.08</t>
-        </is>
+      <c r="B133">
+        <v>10549.347</v>
+      </c>
+      <c r="C133">
+        <v>114.08</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
@@ -3289,15 +2761,11 @@
           <t>GBR</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>67508.936000000002</t>
-        </is>
-      </c>
-      <c r="C134" t="inlineStr">
-        <is>
-          <t>676.88699999999994</t>
-        </is>
+      <c r="B134">
+        <v>67508.936</v>
+      </c>
+      <c r="C134">
+        <v>676.8869999999999</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -3311,15 +2779,11 @@
           <t>ALB</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>2842.3209999999999</t>
-        </is>
-      </c>
-      <c r="C135" t="inlineStr">
-        <is>
-          <t>28.795000000000002</t>
-        </is>
+      <c r="B135">
+        <v>2842.321</v>
+      </c>
+      <c r="C135">
+        <v>28.795</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
@@ -3333,15 +2797,11 @@
           <t>AND</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>79.823999999999998</t>
-        </is>
-      </c>
-      <c r="C136" t="inlineStr">
-        <is>
-          <t>0.57499999999999996</t>
-        </is>
+      <c r="B136">
+        <v>79.824</v>
+      </c>
+      <c r="C136">
+        <v>0.575</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -3355,15 +2815,11 @@
           <t>BIH</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>3233.5259999999998</t>
-        </is>
-      </c>
-      <c r="C137" t="inlineStr">
-        <is>
-          <t>26.763999999999999</t>
-        </is>
+      <c r="B137">
+        <v>3233.526</v>
+      </c>
+      <c r="C137">
+        <v>26.764</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -3377,15 +2833,11 @@
           <t>HRV</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>4030.3580000000002</t>
-        </is>
-      </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>33.923999999999999</t>
-        </is>
+      <c r="B138">
+        <v>4030.358</v>
+      </c>
+      <c r="C138">
+        <v>33.924</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
@@ -3399,15 +2851,11 @@
           <t>GIB</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>32.649000000000001</t>
-        </is>
-      </c>
-      <c r="C139" t="inlineStr">
-        <is>
-          <t>0.34499999999999997</t>
-        </is>
+      <c r="B139">
+        <v>32.649</v>
+      </c>
+      <c r="C139">
+        <v>0.345</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
@@ -3421,15 +2869,11 @@
           <t>GRC</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>10384.971</t>
-        </is>
-      </c>
-      <c r="C140" t="inlineStr">
-        <is>
-          <t>77.141000000000005</t>
-        </is>
+      <c r="B140">
+        <v>10384.971</v>
+      </c>
+      <c r="C140">
+        <v>77.14100000000001</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
@@ -3443,15 +2887,8 @@
           <t>VAT</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>0.51</t>
-        </is>
-      </c>
-      <c r="C141" t="inlineStr">
-        <is>
-          <t>...</t>
-        </is>
+      <c r="B141">
+        <v>0.51</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
@@ -3465,15 +2902,11 @@
           <t>ITA</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>59037.474000000002</t>
-        </is>
-      </c>
-      <c r="C142" t="inlineStr">
-        <is>
-          <t>407.303</t>
-        </is>
+      <c r="B142">
+        <v>59037.474</v>
+      </c>
+      <c r="C142">
+        <v>407.303</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
@@ -3487,15 +2920,11 @@
           <t>XKX</t>
         </is>
       </c>
-      <c r="B143" t="inlineStr">
-        <is>
-          <t>1659.7139999999999</t>
-        </is>
-      </c>
-      <c r="C143" t="inlineStr">
-        <is>
-          <t>18.396999999999998</t>
-        </is>
+      <c r="B143">
+        <v>1659.714</v>
+      </c>
+      <c r="C143">
+        <v>18.397</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
@@ -3509,15 +2938,11 @@
           <t>MLT</t>
         </is>
       </c>
-      <c r="B144" t="inlineStr">
-        <is>
-          <t>533.28599999999994</t>
-        </is>
-      </c>
-      <c r="C144" t="inlineStr">
-        <is>
-          <t>4.8570000000000002</t>
-        </is>
+      <c r="B144">
+        <v>533.2859999999999</v>
+      </c>
+      <c r="C144">
+        <v>4.857</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
@@ -3531,15 +2956,11 @@
           <t>MNE</t>
         </is>
       </c>
-      <c r="B145" t="inlineStr">
-        <is>
-          <t>627.08199999999999</t>
-        </is>
-      </c>
-      <c r="C145" t="inlineStr">
-        <is>
-          <t>6.859</t>
-        </is>
+      <c r="B145">
+        <v>627.082</v>
+      </c>
+      <c r="C145">
+        <v>6.859</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
@@ -3553,15 +2974,11 @@
           <t>MKD</t>
         </is>
       </c>
-      <c r="B146" t="inlineStr">
-        <is>
-          <t>2093.5990000000002</t>
-        </is>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>19.992000000000001</t>
-        </is>
+      <c r="B146">
+        <v>2093.599</v>
+      </c>
+      <c r="C146">
+        <v>19.992</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
@@ -3575,15 +2992,11 @@
           <t>PRT</t>
         </is>
       </c>
-      <c r="B147" t="inlineStr">
-        <is>
-          <t>10270.865</t>
-        </is>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>80.033000000000001</t>
-        </is>
+      <c r="B147">
+        <v>10270.865</v>
+      </c>
+      <c r="C147">
+        <v>80.033</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
@@ -3597,15 +3010,11 @@
           <t>SMR</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>33.659999999999997</t>
-        </is>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
+      <c r="B148">
+        <v>33.66</v>
+      </c>
+      <c r="C148">
+        <v>0.2</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
@@ -3619,15 +3028,11 @@
           <t>SRB</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>7221.3649999999998</t>
-        </is>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>66.557000000000002</t>
-        </is>
+      <c r="B149">
+        <v>7221.365</v>
+      </c>
+      <c r="C149">
+        <v>66.557</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
@@ -3641,15 +3046,11 @@
           <t>SVN</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>2119.8440000000001</t>
-        </is>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>18.835999999999999</t>
-        </is>
+      <c r="B150">
+        <v>2119.844</v>
+      </c>
+      <c r="C150">
+        <v>18.836</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
@@ -3663,15 +3064,11 @@
           <t>ESP</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>47558.63</t>
-        </is>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>356.35899999999998</t>
-        </is>
+      <c r="B151">
+        <v>47558.63</v>
+      </c>
+      <c r="C151">
+        <v>356.359</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
@@ -3685,15 +3082,11 @@
           <t>AUT</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>8939.6170000000002</t>
-        </is>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>84.394000000000005</t>
-        </is>
+      <c r="B152">
+        <v>8939.617</v>
+      </c>
+      <c r="C152">
+        <v>84.39400000000001</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
@@ -3707,15 +3100,11 @@
           <t>BEL</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>11655.93</t>
-        </is>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>117.003</t>
-        </is>
+      <c r="B153">
+        <v>11655.93</v>
+      </c>
+      <c r="C153">
+        <v>117.003</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
@@ -3729,15 +3118,11 @@
           <t>FRA</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>64626.627999999997</t>
-        </is>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>672.88</t>
-        </is>
+      <c r="B154">
+        <v>64626.628</v>
+      </c>
+      <c r="C154">
+        <v>672.88</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
@@ -3751,15 +3136,11 @@
           <t>DEU</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>83369.842999999993</t>
-        </is>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>761.19399999999996</t>
-        </is>
+      <c r="B155">
+        <v>83369.84299999999</v>
+      </c>
+      <c r="C155">
+        <v>761.194</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
@@ -3773,15 +3154,11 @@
           <t>LIE</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>39.326999999999998</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>0.36099999999999999</t>
-        </is>
+      <c r="B156">
+        <v>39.327</v>
+      </c>
+      <c r="C156">
+        <v>0.361</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
@@ -3795,15 +3172,11 @@
           <t>LUX</t>
         </is>
       </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>647.59900000000005</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>6.6749999999999998</t>
-        </is>
+      <c r="B157">
+        <v>647.599</v>
+      </c>
+      <c r="C157">
+        <v>6.675</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
@@ -3817,15 +3190,11 @@
           <t>MCO</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>36.469000000000001</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>0.31900000000000001</t>
-        </is>
+      <c r="B158">
+        <v>36.469</v>
+      </c>
+      <c r="C158">
+        <v>0.319</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
@@ -3839,15 +3208,11 @@
           <t>NLD</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>17564.013999999999</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>181.387</t>
-        </is>
+      <c r="B159">
+        <v>17564.014</v>
+      </c>
+      <c r="C159">
+        <v>181.387</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
@@ -3861,15 +3226,11 @@
           <t>CHE</t>
         </is>
       </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>8740.4719999999998</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>86.478999999999999</t>
-        </is>
+      <c r="B160">
+        <v>8740.472</v>
+      </c>
+      <c r="C160">
+        <v>86.479</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
@@ -3883,15 +3244,11 @@
           <t>AIA</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>15.856999999999999</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
+      <c r="B161">
+        <v>15.857</v>
+      </c>
+      <c r="C161">
+        <v>0.15</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
@@ -3905,15 +3262,11 @@
           <t>ATG</t>
         </is>
       </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>93.763000000000005</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>1.1240000000000001</t>
-        </is>
+      <c r="B162">
+        <v>93.76300000000001</v>
+      </c>
+      <c r="C162">
+        <v>1.124</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
@@ -3927,15 +3280,11 @@
           <t>ABW</t>
         </is>
       </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>106.44499999999999</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>0.76300000000000001</t>
-        </is>
+      <c r="B163">
+        <v>106.445</v>
+      </c>
+      <c r="C163">
+        <v>0.763</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
@@ -3949,15 +3298,11 @@
           <t>BHS</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>409.98399999999998</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>4.6589999999999998</t>
-        </is>
+      <c r="B164">
+        <v>409.984</v>
+      </c>
+      <c r="C164">
+        <v>4.659</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
@@ -3971,15 +3316,11 @@
           <t>BRB</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>281.63499999999999</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>3.0369999999999999</t>
-        </is>
+      <c r="B165">
+        <v>281.635</v>
+      </c>
+      <c r="C165">
+        <v>3.037</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
@@ -3993,15 +3334,11 @@
           <t>BES</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>27.026</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>0.28699999999999998</t>
-        </is>
+      <c r="B166">
+        <v>27.026</v>
+      </c>
+      <c r="C166">
+        <v>0.287</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
@@ -4015,15 +3352,11 @@
           <t>VGB</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>31.305</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>0.23799999999999999</t>
-        </is>
+      <c r="B167">
+        <v>31.305</v>
+      </c>
+      <c r="C167">
+        <v>0.238</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
@@ -4037,15 +3370,11 @@
           <t>CYM</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>68.706000000000003</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>0.66900000000000004</t>
-        </is>
+      <c r="B168">
+        <v>68.706</v>
+      </c>
+      <c r="C168">
+        <v>0.669</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
@@ -4059,15 +3388,11 @@
           <t>CUB</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>11212.191000000001</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>99.692999999999998</t>
-        </is>
+      <c r="B169">
+        <v>11212.191</v>
+      </c>
+      <c r="C169">
+        <v>99.693</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
@@ -4081,15 +3406,11 @@
           <t>CUW</t>
         </is>
       </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>191.16300000000001</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>2.1829999999999998</t>
-        </is>
+      <c r="B170">
+        <v>191.163</v>
+      </c>
+      <c r="C170">
+        <v>2.183</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
@@ -4103,15 +3424,11 @@
           <t>DMA</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>72.736999999999995</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>0.96599999999999997</t>
-        </is>
+      <c r="B171">
+        <v>72.73699999999999</v>
+      </c>
+      <c r="C171">
+        <v>0.966</v>
       </c>
       <c r="D171" t="inlineStr">
         <is>
@@ -4125,15 +3442,11 @@
           <t>DOM</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>11228.821</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>203.625</t>
-        </is>
+      <c r="B172">
+        <v>11228.821</v>
+      </c>
+      <c r="C172">
+        <v>203.625</v>
       </c>
       <c r="D172" t="inlineStr">
         <is>
@@ -4147,15 +3460,11 @@
           <t>GRD</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>125.438</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>1.96</t>
-        </is>
+      <c r="B173">
+        <v>125.438</v>
+      </c>
+      <c r="C173">
+        <v>1.96</v>
       </c>
       <c r="D173" t="inlineStr">
         <is>
@@ -4169,15 +3478,11 @@
           <t>GLP</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>395.75200000000001</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>4.5179999999999998</t>
-        </is>
+      <c r="B174">
+        <v>395.752</v>
+      </c>
+      <c r="C174">
+        <v>4.518</v>
       </c>
       <c r="D174" t="inlineStr">
         <is>
@@ -4191,15 +3496,11 @@
           <t>HTI</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>11584.995999999999</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>268.52300000000002</t>
-        </is>
+      <c r="B175">
+        <v>11584.996</v>
+      </c>
+      <c r="C175">
+        <v>268.523</v>
       </c>
       <c r="D175" t="inlineStr">
         <is>
@@ -4213,15 +3514,11 @@
           <t>JAM</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>2827.377</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>32.662999999999997</t>
-        </is>
+      <c r="B176">
+        <v>2827.377</v>
+      </c>
+      <c r="C176">
+        <v>32.663</v>
       </c>
       <c r="D176" t="inlineStr">
         <is>
@@ -4235,15 +3532,11 @@
           <t>MTQ</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>367.50700000000001</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>3.508</t>
-        </is>
+      <c r="B177">
+        <v>367.507</v>
+      </c>
+      <c r="C177">
+        <v>3.508</v>
       </c>
       <c r="D177" t="inlineStr">
         <is>
@@ -4257,15 +3550,11 @@
           <t>MSR</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>4.3899999999999997</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>0.04</t>
-        </is>
+      <c r="B178">
+        <v>4.39</v>
+      </c>
+      <c r="C178">
+        <v>0.04</v>
       </c>
       <c r="D178" t="inlineStr">
         <is>
@@ -4279,15 +3568,11 @@
           <t>PRI</t>
         </is>
       </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>3252.4070000000002</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>26.058</t>
-        </is>
+      <c r="B179">
+        <v>3252.407</v>
+      </c>
+      <c r="C179">
+        <v>26.058</v>
       </c>
       <c r="D179" t="inlineStr">
         <is>
@@ -4301,15 +3586,11 @@
           <t>BLM</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>10.967000000000001</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>9.1999999999999998E-2</t>
-        </is>
+      <c r="B180">
+        <v>10.967</v>
+      </c>
+      <c r="C180">
+        <v>0.092</v>
       </c>
       <c r="D180" t="inlineStr">
         <is>
@@ -4323,15 +3604,11 @@
           <t>KNA</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>47.656999999999996</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>0.56299999999999994</t>
-        </is>
+      <c r="B181">
+        <v>47.657</v>
+      </c>
+      <c r="C181">
+        <v>0.5629999999999999</v>
       </c>
       <c r="D181" t="inlineStr">
         <is>
@@ -4345,15 +3622,11 @@
           <t>LCA</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>179.857</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>2.0350000000000001</t>
-        </is>
+      <c r="B182">
+        <v>179.857</v>
+      </c>
+      <c r="C182">
+        <v>2.035</v>
       </c>
       <c r="D182" t="inlineStr">
         <is>
@@ -4367,15 +3640,11 @@
           <t>MAF</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>31.791</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>0.45800000000000002</t>
-        </is>
+      <c r="B183">
+        <v>31.791</v>
+      </c>
+      <c r="C183">
+        <v>0.458</v>
       </c>
       <c r="D183" t="inlineStr">
         <is>
@@ -4389,15 +3658,11 @@
           <t>VCT</t>
         </is>
       </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>103.94799999999999</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>1.3240000000000001</t>
-        </is>
+      <c r="B184">
+        <v>103.948</v>
+      </c>
+      <c r="C184">
+        <v>1.324</v>
       </c>
       <c r="D184" t="inlineStr">
         <is>
@@ -4411,15 +3676,11 @@
           <t>SXM</t>
         </is>
       </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>44.174999999999997</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>0.36</t>
-        </is>
+      <c r="B185">
+        <v>44.175</v>
+      </c>
+      <c r="C185">
+        <v>0.36</v>
       </c>
       <c r="D185" t="inlineStr">
         <is>
@@ -4433,15 +3694,11 @@
           <t>TTO</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>1531.0440000000001</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>17.428999999999998</t>
-        </is>
+      <c r="B186">
+        <v>1531.044</v>
+      </c>
+      <c r="C186">
+        <v>17.429</v>
       </c>
       <c r="D186" t="inlineStr">
         <is>
@@ -4455,15 +3712,11 @@
           <t>TCA</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>45.703000000000003</t>
-        </is>
-      </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>0.56000000000000005</t>
-        </is>
+      <c r="B187">
+        <v>45.703</v>
+      </c>
+      <c r="C187">
+        <v>0.5600000000000001</v>
       </c>
       <c r="D187" t="inlineStr">
         <is>
@@ -4477,15 +3730,11 @@
           <t>VIR</t>
         </is>
       </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>99.465000000000003</t>
-        </is>
-      </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>1.1180000000000001</t>
-        </is>
+      <c r="B188">
+        <v>99.465</v>
+      </c>
+      <c r="C188">
+        <v>1.118</v>
       </c>
       <c r="D188" t="inlineStr">
         <is>
@@ -4499,15 +3748,11 @@
           <t>BLZ</t>
         </is>
       </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>405.27199999999999</t>
-        </is>
-      </c>
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>7.1929999999999996</t>
-        </is>
+      <c r="B189">
+        <v>405.272</v>
+      </c>
+      <c r="C189">
+        <v>7.193</v>
       </c>
       <c r="D189" t="inlineStr">
         <is>
@@ -4521,15 +3766,11 @@
           <t>CRI</t>
         </is>
       </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>5180.8289999999997</t>
-        </is>
-      </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>60.517000000000003</t>
-        </is>
+      <c r="B190">
+        <v>5180.829</v>
+      </c>
+      <c r="C190">
+        <v>60.517</v>
       </c>
       <c r="D190" t="inlineStr">
         <is>
@@ -4543,15 +3784,11 @@
           <t>SLV</t>
         </is>
       </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>6336.3919999999998</t>
-        </is>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>100.313</t>
-        </is>
+      <c r="B191">
+        <v>6336.392</v>
+      </c>
+      <c r="C191">
+        <v>100.313</v>
       </c>
       <c r="D191" t="inlineStr">
         <is>
@@ -4565,15 +3802,11 @@
           <t>GTM</t>
         </is>
       </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>17843.907999999999</t>
-        </is>
-      </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>372.33499999999998</t>
-        </is>
+      <c r="B192">
+        <v>17843.908</v>
+      </c>
+      <c r="C192">
+        <v>372.335</v>
       </c>
       <c r="D192" t="inlineStr">
         <is>
@@ -4587,15 +3820,11 @@
           <t>HND</t>
         </is>
       </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>10432.86</t>
-        </is>
-      </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>217.59</t>
-        </is>
+      <c r="B193">
+        <v>10432.86</v>
+      </c>
+      <c r="C193">
+        <v>217.59</v>
       </c>
       <c r="D193" t="inlineStr">
         <is>
@@ -4609,15 +3838,11 @@
           <t>MEX</t>
         </is>
       </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>127504.125</t>
-        </is>
-      </c>
-      <c r="C194" t="inlineStr">
-        <is>
-          <t>1866.3989999999999</t>
-        </is>
+      <c r="B194">
+        <v>127504.125</v>
+      </c>
+      <c r="C194">
+        <v>1866.399</v>
       </c>
       <c r="D194" t="inlineStr">
         <is>
@@ -4631,15 +3856,11 @@
           <t>NIC</t>
         </is>
       </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>6948.3919999999998</t>
-        </is>
-      </c>
-      <c r="C195" t="inlineStr">
-        <is>
-          <t>139.16399999999999</t>
-        </is>
+      <c r="B195">
+        <v>6948.392</v>
+      </c>
+      <c r="C195">
+        <v>139.164</v>
       </c>
       <c r="D195" t="inlineStr">
         <is>
@@ -4653,15 +3874,11 @@
           <t>PAN</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>4408.5810000000001</t>
-        </is>
-      </c>
-      <c r="C196" t="inlineStr">
-        <is>
-          <t>76.637</t>
-        </is>
+      <c r="B196">
+        <v>4408.581</v>
+      </c>
+      <c r="C196">
+        <v>76.637</v>
       </c>
       <c r="D196" t="inlineStr">
         <is>
@@ -4675,15 +3892,11 @@
           <t>ARG</t>
         </is>
       </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>45510.317999999999</t>
-        </is>
-      </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>627.74099999999999</t>
-        </is>
+      <c r="B197">
+        <v>45510.318</v>
+      </c>
+      <c r="C197">
+        <v>627.741</v>
       </c>
       <c r="D197" t="inlineStr">
         <is>
@@ -4697,15 +3910,11 @@
           <t>BOL</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>12224.11</t>
-        </is>
-      </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>264.07</t>
-        </is>
+      <c r="B198">
+        <v>12224.11</v>
+      </c>
+      <c r="C198">
+        <v>264.07</v>
       </c>
       <c r="D198" t="inlineStr">
         <is>
@@ -4719,15 +3928,11 @@
           <t>BRA</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>215313.49799999999</t>
-        </is>
-      </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>2723.2660000000001</t>
-        </is>
+      <c r="B199">
+        <v>215313.498</v>
+      </c>
+      <c r="C199">
+        <v>2723.266</v>
       </c>
       <c r="D199" t="inlineStr">
         <is>
@@ -4741,15 +3946,11 @@
           <t>CHL</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>19603.733</t>
-        </is>
-      </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>230.82400000000001</t>
-        </is>
+      <c r="B200">
+        <v>19603.733</v>
+      </c>
+      <c r="C200">
+        <v>230.824</v>
       </c>
       <c r="D200" t="inlineStr">
         <is>
@@ -4763,15 +3964,11 @@
           <t>COL</t>
         </is>
       </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>51874.023999999998</t>
-        </is>
-      </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>723.26400000000001</t>
-        </is>
+      <c r="B201">
+        <v>51874.024</v>
+      </c>
+      <c r="C201">
+        <v>723.264</v>
       </c>
       <c r="D201" t="inlineStr">
         <is>
@@ -4785,15 +3982,11 @@
           <t>ECU</t>
         </is>
       </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>18001</t>
-        </is>
-      </c>
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>298.666</t>
-        </is>
+      <c r="B202">
+        <v>18001</v>
+      </c>
+      <c r="C202">
+        <v>298.666</v>
       </c>
       <c r="D202" t="inlineStr">
         <is>
@@ -4807,15 +4000,11 @@
           <t>FLK</t>
         </is>
       </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>3.78</t>
-        </is>
-      </c>
-      <c r="C203" t="inlineStr">
-        <is>
-          <t>4.2000000000000003E-2</t>
-        </is>
+      <c r="B203">
+        <v>3.78</v>
+      </c>
+      <c r="C203">
+        <v>0.042</v>
       </c>
       <c r="D203" t="inlineStr">
         <is>
@@ -4829,15 +4018,11 @@
           <t>GUF</t>
         </is>
       </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>304.55700000000002</t>
-        </is>
-      </c>
-      <c r="C204" t="inlineStr">
-        <is>
-          <t>7.5730000000000004</t>
-        </is>
+      <c r="B204">
+        <v>304.557</v>
+      </c>
+      <c r="C204">
+        <v>7.573</v>
       </c>
       <c r="D204" t="inlineStr">
         <is>
@@ -4851,15 +4036,11 @@
           <t>GUY</t>
         </is>
       </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>808.726</t>
-        </is>
-      </c>
-      <c r="C205" t="inlineStr">
-        <is>
-          <t>16.129000000000001</t>
-        </is>
+      <c r="B205">
+        <v>808.726</v>
+      </c>
+      <c r="C205">
+        <v>16.129</v>
       </c>
       <c r="D205" t="inlineStr">
         <is>
@@ -4873,15 +4054,11 @@
           <t>PRY</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>6780.7439999999997</t>
-        </is>
-      </c>
-      <c r="C206" t="inlineStr">
-        <is>
-          <t>137.96</t>
-        </is>
+      <c r="B206">
+        <v>6780.744</v>
+      </c>
+      <c r="C206">
+        <v>137.96</v>
       </c>
       <c r="D206" t="inlineStr">
         <is>
@@ -4895,15 +4072,11 @@
           <t>PER</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>34049.588000000003</t>
-        </is>
-      </c>
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>592.15599999999995</t>
-        </is>
+      <c r="B207">
+        <v>34049.588</v>
+      </c>
+      <c r="C207">
+        <v>592.1559999999999</v>
       </c>
       <c r="D207" t="inlineStr">
         <is>
@@ -4917,15 +4090,11 @@
           <t>SUR</t>
         </is>
       </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>618.04</t>
-        </is>
-      </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>11.122999999999999</t>
-        </is>
+      <c r="B208">
+        <v>618.04</v>
+      </c>
+      <c r="C208">
+        <v>11.123</v>
       </c>
       <c r="D208" t="inlineStr">
         <is>
@@ -4939,15 +4108,11 @@
           <t>URY</t>
         </is>
       </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>3422.7939999999999</t>
-        </is>
-      </c>
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>35.667999999999999</t>
-        </is>
+      <c r="B209">
+        <v>3422.794</v>
+      </c>
+      <c r="C209">
+        <v>35.668</v>
       </c>
       <c r="D209" t="inlineStr">
         <is>
@@ -4961,15 +4126,11 @@
           <t>VEN</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>28301.696</t>
-        </is>
-      </c>
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>438.38400000000001</t>
-        </is>
+      <c r="B210">
+        <v>28301.696</v>
+      </c>
+      <c r="C210">
+        <v>438.384</v>
       </c>
       <c r="D210" t="inlineStr">
         <is>
@@ -4983,15 +4144,11 @@
           <t>BMU</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>64.183999999999997</t>
-        </is>
-      </c>
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>0.48199999999999998</t>
-        </is>
+      <c r="B211">
+        <v>64.184</v>
+      </c>
+      <c r="C211">
+        <v>0.482</v>
       </c>
       <c r="D211" t="inlineStr">
         <is>
@@ -5005,15 +4162,11 @@
           <t>CAN</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>38454.326999999997</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>376.18799999999999</t>
-        </is>
+      <c r="B212">
+        <v>38454.327</v>
+      </c>
+      <c r="C212">
+        <v>376.188</v>
       </c>
       <c r="D212" t="inlineStr">
         <is>
@@ -5027,15 +4180,11 @@
           <t>GRL</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>56.466000000000001</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>0.79600000000000004</t>
-        </is>
+      <c r="B213">
+        <v>56.466</v>
+      </c>
+      <c r="C213">
+        <v>0.796</v>
       </c>
       <c r="D213" t="inlineStr">
         <is>
@@ -5049,15 +4198,11 @@
           <t>SPM</t>
         </is>
       </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>5.8620000000000001</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>4.3999999999999997E-2</t>
-        </is>
+      <c r="B214">
+        <v>5.862</v>
+      </c>
+      <c r="C214">
+        <v>0.044</v>
       </c>
       <c r="D214" t="inlineStr">
         <is>
@@ -5071,15 +4216,11 @@
           <t>USA</t>
         </is>
       </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>338289.85700000002</t>
-        </is>
-      </c>
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>3726.8670000000002</t>
-        </is>
+      <c r="B215">
+        <v>338289.857</v>
+      </c>
+      <c r="C215">
+        <v>3726.867</v>
       </c>
       <c r="D215" t="inlineStr">
         <is>
@@ -5093,15 +4234,11 @@
           <t>AUS</t>
         </is>
       </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>26177.413</t>
-        </is>
-      </c>
-      <c r="C216" t="inlineStr">
-        <is>
-          <t>300.24599999999998</t>
-        </is>
+      <c r="B216">
+        <v>26177.413</v>
+      </c>
+      <c r="C216">
+        <v>300.246</v>
       </c>
       <c r="D216" t="inlineStr">
         <is>
@@ -5115,15 +4252,11 @@
           <t>NZL</t>
         </is>
       </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>5185.2879999999996</t>
-        </is>
-      </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>64.102999999999994</t>
-        </is>
+      <c r="B217">
+        <v>5185.288</v>
+      </c>
+      <c r="C217">
+        <v>64.10299999999999</v>
       </c>
       <c r="D217" t="inlineStr">
         <is>
@@ -5137,15 +4270,11 @@
           <t>FJI</t>
         </is>
       </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>929.76599999999996</t>
-        </is>
-      </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>17.821000000000002</t>
-        </is>
+      <c r="B218">
+        <v>929.766</v>
+      </c>
+      <c r="C218">
+        <v>17.821</v>
       </c>
       <c r="D218" t="inlineStr">
         <is>
@@ -5159,15 +4288,11 @@
           <t>NCL</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>289.95</t>
-        </is>
-      </c>
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>4.0949999999999998</t>
-        </is>
+      <c r="B219">
+        <v>289.95</v>
+      </c>
+      <c r="C219">
+        <v>4.095</v>
       </c>
       <c r="D219" t="inlineStr">
         <is>
@@ -5181,15 +4306,11 @@
           <t>PNG</t>
         </is>
       </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>10142.619000000001</t>
-        </is>
-      </c>
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>254.71799999999999</t>
-        </is>
+      <c r="B220">
+        <v>10142.619</v>
+      </c>
+      <c r="C220">
+        <v>254.718</v>
       </c>
       <c r="D220" t="inlineStr">
         <is>
@@ -5203,15 +4324,11 @@
           <t>SLB</t>
         </is>
       </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>724.27300000000002</t>
-        </is>
-      </c>
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>21.262</t>
-        </is>
+      <c r="B221">
+        <v>724.273</v>
+      </c>
+      <c r="C221">
+        <v>21.262</v>
       </c>
       <c r="D221" t="inlineStr">
         <is>
@@ -5225,15 +4342,11 @@
           <t>VUT</t>
         </is>
       </c>
-      <c r="B222" t="inlineStr">
-        <is>
-          <t>326.74</t>
-        </is>
-      </c>
-      <c r="C222" t="inlineStr">
-        <is>
-          <t>9.4659999999999993</t>
-        </is>
+      <c r="B222">
+        <v>326.74</v>
+      </c>
+      <c r="C222">
+        <v>9.465999999999999</v>
       </c>
       <c r="D222" t="inlineStr">
         <is>
@@ -5247,15 +4360,11 @@
           <t>GUM</t>
         </is>
       </c>
-      <c r="B223" t="inlineStr">
-        <is>
-          <t>171.774</t>
-        </is>
-      </c>
-      <c r="C223" t="inlineStr">
-        <is>
-          <t>2.8170000000000002</t>
-        </is>
+      <c r="B223">
+        <v>171.774</v>
+      </c>
+      <c r="C223">
+        <v>2.817</v>
       </c>
       <c r="D223" t="inlineStr">
         <is>
@@ -5269,15 +4378,11 @@
           <t>KIR</t>
         </is>
       </c>
-      <c r="B224" t="inlineStr">
-        <is>
-          <t>131.232</t>
-        </is>
-      </c>
-      <c r="C224" t="inlineStr">
-        <is>
-          <t>3.512</t>
-        </is>
+      <c r="B224">
+        <v>131.232</v>
+      </c>
+      <c r="C224">
+        <v>3.512</v>
       </c>
       <c r="D224" t="inlineStr">
         <is>
@@ -5291,15 +4396,11 @@
           <t>MHL</t>
         </is>
       </c>
-      <c r="B225" t="inlineStr">
-        <is>
-          <t>41.569000000000003</t>
-        </is>
-      </c>
-      <c r="C225" t="inlineStr">
-        <is>
-          <t>0.77</t>
-        </is>
+      <c r="B225">
+        <v>41.569</v>
+      </c>
+      <c r="C225">
+        <v>0.77</v>
       </c>
       <c r="D225" t="inlineStr">
         <is>
@@ -5313,15 +4414,11 @@
           <t>FSM</t>
         </is>
       </c>
-      <c r="B226" t="inlineStr">
-        <is>
-          <t>114.164</t>
-        </is>
-      </c>
-      <c r="C226" t="inlineStr">
-        <is>
-          <t>2.3679999999999999</t>
-        </is>
+      <c r="B226">
+        <v>114.164</v>
+      </c>
+      <c r="C226">
+        <v>2.368</v>
       </c>
       <c r="D226" t="inlineStr">
         <is>
@@ -5335,15 +4432,11 @@
           <t>NRU</t>
         </is>
       </c>
-      <c r="B227" t="inlineStr">
-        <is>
-          <t>12.667999999999999</t>
-        </is>
-      </c>
-      <c r="C227" t="inlineStr">
-        <is>
-          <t>0.34100000000000003</t>
-        </is>
+      <c r="B227">
+        <v>12.668</v>
+      </c>
+      <c r="C227">
+        <v>0.341</v>
       </c>
       <c r="D227" t="inlineStr">
         <is>
@@ -5357,15 +4450,11 @@
           <t>MNP</t>
         </is>
       </c>
-      <c r="B228" t="inlineStr">
-        <is>
-          <t>49.551000000000002</t>
-        </is>
-      </c>
-      <c r="C228" t="inlineStr">
-        <is>
-          <t>0.60399999999999998</t>
-        </is>
+      <c r="B228">
+        <v>49.551</v>
+      </c>
+      <c r="C228">
+        <v>0.604</v>
       </c>
       <c r="D228" t="inlineStr">
         <is>
@@ -5379,15 +4468,11 @@
           <t>PLW</t>
         </is>
       </c>
-      <c r="B229" t="inlineStr">
-        <is>
-          <t>18.055</t>
-        </is>
-      </c>
-      <c r="C229" t="inlineStr">
-        <is>
-          <t>0.27</t>
-        </is>
+      <c r="B229">
+        <v>18.055</v>
+      </c>
+      <c r="C229">
+        <v>0.27</v>
       </c>
       <c r="D229" t="inlineStr">
         <is>
@@ -5401,15 +4486,11 @@
           <t>ASM</t>
         </is>
       </c>
-      <c r="B230" t="inlineStr">
-        <is>
-          <t>44.273000000000003</t>
-        </is>
-      </c>
-      <c r="C230" t="inlineStr">
-        <is>
-          <t>0.76500000000000001</t>
-        </is>
+      <c r="B230">
+        <v>44.273</v>
+      </c>
+      <c r="C230">
+        <v>0.765</v>
       </c>
       <c r="D230" t="inlineStr">
         <is>
@@ -5423,15 +4504,11 @@
           <t>COK</t>
         </is>
       </c>
-      <c r="B231" t="inlineStr">
-        <is>
-          <t>17.010999999999999</t>
-        </is>
-      </c>
-      <c r="C231" t="inlineStr">
-        <is>
-          <t>0.27500000000000002</t>
-        </is>
+      <c r="B231">
+        <v>17.011</v>
+      </c>
+      <c r="C231">
+        <v>0.275</v>
       </c>
       <c r="D231" t="inlineStr">
         <is>
@@ -5445,15 +4522,11 @@
           <t>PYF</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>306.279</t>
-        </is>
-      </c>
-      <c r="C232" t="inlineStr">
-        <is>
-          <t>3.8439999999999999</t>
-        </is>
+      <c r="B232">
+        <v>306.279</v>
+      </c>
+      <c r="C232">
+        <v>3.844</v>
       </c>
       <c r="D232" t="inlineStr">
         <is>
@@ -5467,15 +4540,11 @@
           <t>NIU</t>
         </is>
       </c>
-      <c r="B233" t="inlineStr">
-        <is>
-          <t>1.9339999999999999</t>
-        </is>
-      </c>
-      <c r="C233" t="inlineStr">
-        <is>
-          <t>2.7E-2</t>
-        </is>
+      <c r="B233">
+        <v>1.934</v>
+      </c>
+      <c r="C233">
+        <v>0.027</v>
       </c>
       <c r="D233" t="inlineStr">
         <is>
@@ -5489,15 +4558,11 @@
           <t>WSM</t>
         </is>
       </c>
-      <c r="B234" t="inlineStr">
-        <is>
-          <t>222.38200000000001</t>
-        </is>
-      </c>
-      <c r="C234" t="inlineStr">
-        <is>
-          <t>6.024</t>
-        </is>
+      <c r="B234">
+        <v>222.382</v>
+      </c>
+      <c r="C234">
+        <v>6.024</v>
       </c>
       <c r="D234" t="inlineStr">
         <is>
@@ -5511,15 +4576,11 @@
           <t>TKL</t>
         </is>
       </c>
-      <c r="B235" t="inlineStr">
-        <is>
-          <t>1.871</t>
-        </is>
-      </c>
-      <c r="C235" t="inlineStr">
-        <is>
-          <t>3.5000000000000003E-2</t>
-        </is>
+      <c r="B235">
+        <v>1.871</v>
+      </c>
+      <c r="C235">
+        <v>0.035</v>
       </c>
       <c r="D235" t="inlineStr">
         <is>
@@ -5533,15 +4594,11 @@
           <t>TON</t>
         </is>
       </c>
-      <c r="B236" t="inlineStr">
-        <is>
-          <t>106.858</t>
-        </is>
-      </c>
-      <c r="C236" t="inlineStr">
-        <is>
-          <t>2.456</t>
-        </is>
+      <c r="B236">
+        <v>106.858</v>
+      </c>
+      <c r="C236">
+        <v>2.456</v>
       </c>
       <c r="D236" t="inlineStr">
         <is>
@@ -5555,15 +4612,11 @@
           <t>TUV</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>11.311999999999999</t>
-        </is>
-      </c>
-      <c r="C237" t="inlineStr">
-        <is>
-          <t>0.26500000000000001</t>
-        </is>
+      <c r="B237">
+        <v>11.312</v>
+      </c>
+      <c r="C237">
+        <v>0.265</v>
       </c>
       <c r="D237" t="inlineStr">
         <is>
@@ -5577,15 +4630,11 @@
           <t>WLF</t>
         </is>
       </c>
-      <c r="B238" t="inlineStr">
-        <is>
-          <t>11.571999999999999</t>
-        </is>
-      </c>
-      <c r="C238" t="inlineStr">
-        <is>
-          <t>0.13500000000000001</t>
-        </is>
+      <c r="B238">
+        <v>11.572</v>
+      </c>
+      <c r="C238">
+        <v>0.135</v>
       </c>
       <c r="D238" t="inlineStr">
         <is>

</xml_diff>